<commit_message>
added database connection and made user model
</commit_message>
<xml_diff>
--- a/public/upload-Tarik.xlsx
+++ b/public/upload-Tarik.xlsx
@@ -16,7 +16,6 @@
 <office:document-content xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:rpt="http://openoffice.org/2005/report" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:xforms="http://www.w3.org/2002/xforms" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:formx="urn:openoffice:names:experimental:ooxml-odf-interop:xmlns:form:1.0" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" office:version="1.3">
   <office:scripts/>
   <office:font-face-decls>
-    <style:font-face style:name="Liberation Serif" svg:font-family="'Liberation Serif'" style:font-family-generic="roman" style:font-pitch="variable"/>
     <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
     <style:font-face style:name="Lucida Sans" svg:font-family="'Lucida Sans'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Mangal" svg:font-family="Mangal" style:font-family-generic="system" style:font-pitch="variable"/>
@@ -132,6 +131,56 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:a xlink:href="mailto:nekonekic@gmail.com" xlink:type="simple">nekonekic@gmail.com</text:a>
+            </text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Admir besic</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:a xlink:href="mailto:admirbesa@gmail.com" xlink:type="simple">admirbesa@gmail.com</text:a>
+            </text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>rijad dervisevic</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:a xlink:href="mailto:rijaddervisevic@gmail.com" xlink:type="simple">rijaddervisevic@gmail.com</text:a>
+            </text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>admiral spider</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:a xlink:href="mailto:admiralspider@gmail.com" xlink:type="simple">admiralspider@gmail.com</text:a>
+            </text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>test test</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:a xlink:href="mailto:test123@gmail.com" xlink:type="simple">test123@gmail.com</text:a>
+            </text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>test2 test2</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:a xlink:href="mailto:test222@gmail.com" xlink:type="simple">test222@gmail.com</text:a>
             </text:p>
           </table:table-cell>
         </table:table-row>
@@ -147,10 +196,10 @@
   <office:meta>
     <meta:creation-date>2017-10-20T23:41:04.964000000</meta:creation-date>
     <meta:generator>LibreOffice/7.0.6.2$Windows_X86_64 LibreOffice_project/144abb84a525d8e30c9dbbefa69cbbf2d8d4ae3b</meta:generator>
-    <dc:date>2021-08-19T15:24:05.086000000</dc:date>
-    <meta:editing-duration>PT25M57S</meta:editing-duration>
-    <meta:editing-cycles>7</meta:editing-cycles>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="18" meta:object-count="0"/>
+    <dc:date>2021-08-21T19:28:30.765000000</dc:date>
+    <meta:editing-duration>PT27M8S</meta:editing-duration>
+    <meta:editing-cycles>12</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="28" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -162,14 +211,14 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">8385</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">4064</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">6321</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">8</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">13</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -187,7 +236,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">Sheet1</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1856</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">957</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -265,7 +314,6 @@
 <file path=styles.xml><?xml version="1.0" encoding="utf-8"?>
 <office:document-styles xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:rpt="http://openoffice.org/2005/report" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" office:version="1.3">
   <office:font-face-decls>
-    <style:font-face style:name="Liberation Serif" svg:font-family="'Liberation Serif'" style:font-family-generic="roman" style:font-pitch="variable"/>
     <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
     <style:font-face style:name="Lucida Sans" svg:font-family="'Lucida Sans'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Mangal" svg:font-family="Mangal" style:font-family-generic="system" style:font-pitch="variable"/>
@@ -395,9 +443,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2021-08-19">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2021-08-21">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="15:21:30.167000000">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="19:28:23.871000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>